<commit_message>
Feito eliminação de gauss
</commit_message>
<xml_diff>
--- a/matriz.xlsx
+++ b/matriz.xlsx
@@ -20,13 +20,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -62,9 +68,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -372,48 +381,58 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D1" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="C1" s="1">
-        <v>7</v>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
         <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feito iterações de gauss
</commit_message>
<xml_diff>
--- a/matriz.xlsx
+++ b/matriz.xlsx
@@ -64,10 +64,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -372,7 +372,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -381,39 +381,63 @@
     <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1">
+        <v>-2</v>
+      </c>
+      <c r="D1" s="1">
         <v>4</v>
-      </c>
-      <c r="B1" s="1">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1">
-        <v>-16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>-43</v>
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>-43</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>98</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>